<commit_message>
-Added Basic Project Structure
</commit_message>
<xml_diff>
--- a/Docs/Projektstrukturplan.xlsx
+++ b/Docs/Projektstrukturplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepos\EscapeTheLore\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD06ED1-E189-4B9A-87F3-DBE4B7269066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F5FC5B-A7C0-4481-A5C5-93C6D2D32B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{71C39013-33C7-429B-B64D-557120CFD4CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>1. Projektmanagement</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>* Item und Pickups</t>
-  </si>
-  <si>
-    <t>* Menü</t>
   </si>
   <si>
     <t>* Spielertextur</t>
@@ -212,9 +209,6 @@
     </r>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">® </t>
     </r>
@@ -297,21 +291,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">® </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Hauptmenü beim Spielstart ("Starten", "Beenden" , "Einstellungen")</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -459,6 +438,84 @@
   </si>
   <si>
     <t>1.8.2 Halbwegspräsentation</t>
+  </si>
+  <si>
+    <t>* Basic-Menü</t>
+  </si>
+  <si>
+    <r>
+      <t>® E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>infaches Starten und beenden des Spiels</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Advanced-Menü</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">® </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spiel Fortsetzen &amp; Neues Spiel erstellen (DB)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Design-Menü</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">® </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Voll Designetes Menü mit Einstellungen &amp; Global-Shop</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -608,12 +665,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -621,15 +677,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -648,9 +704,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -688,7 +744,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -794,7 +850,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -936,7 +992,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -944,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1548ACB-B1BA-42B9-B61E-5213C2AFF6A0}">
-  <dimension ref="A2:H57"/>
+  <dimension ref="A2:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C39" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -960,350 +1016,372 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="14.4" customHeight="1">
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="14.4" customHeight="1">
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="9"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="4.5" customHeight="1">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="8"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="8"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="8"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="E8" s="6" t="s">
+      <c r="A8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="E8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.7">
-      <c r="A10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="E10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="7"/>
+      <c r="A10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="E10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="14.7">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="G11" s="5" t="s">
+      <c r="E11" s="10"/>
+      <c r="G11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="7"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="6"/>
       <c r="E12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="17.100000000000001">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.7">
+      <c r="A14" s="6"/>
+      <c r="E14" s="10"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="14.7">
+      <c r="A16" s="6"/>
+      <c r="E16" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.7">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="G17" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.7">
+      <c r="A18" s="6"/>
+      <c r="E18" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.7">
+      <c r="A19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.7">
+      <c r="A20" s="2"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" ht="14.7">
+      <c r="A21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="14.7">
-      <c r="A14" s="7"/>
-      <c r="E14" s="12"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="14.7">
-      <c r="A16" s="7"/>
-      <c r="E16" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14.7">
-      <c r="A17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="G17" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="7"/>
-      <c r="E18" s="6" t="s">
+      <c r="E21" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.7">
+      <c r="A22" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.7">
+      <c r="A23" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="17.100000000000001">
-      <c r="A19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="14.7">
-      <c r="A22" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17.100000000000001">
       <c r="A25" s="2"/>
-      <c r="E25" s="11" t="s">
-        <v>57</v>
+      <c r="E25" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="E26" s="6"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14.7">
+      <c r="E28" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="E30" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17.100000000000001">
+      <c r="E31" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="E28" s="6" t="s">
+    <row r="34" spans="5:5">
+      <c r="E34" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" ht="17.100000000000001">
+      <c r="E36" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5">
+      <c r="E39" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="E29" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="17.100000000000001">
-      <c r="E30" s="11" t="s">
+    <row r="41" spans="5:5">
+      <c r="E41" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="5:5">
+      <c r="E43" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5">
+      <c r="E44" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" ht="14.7">
+      <c r="E45" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="E32" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5">
-      <c r="E33" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5">
-      <c r="E34" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="5:5">
-      <c r="E35" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="5:5">
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="5:5">
-      <c r="E37" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="5:5">
-      <c r="E38" s="6" t="s">
+    <row r="46" spans="5:5" ht="14.7">
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="5:5">
+      <c r="E47" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="5:5" ht="14.7">
-      <c r="E39" s="12" t="s">
+    <row r="48" spans="5:5" ht="14.7">
+      <c r="E48" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="5:5" ht="14.7">
-      <c r="E40" s="12"/>
-    </row>
-    <row r="41" spans="5:5">
-      <c r="E41" s="6" t="s">
+    <row r="49" spans="5:5" ht="14.7">
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="5:5" ht="14.7">
-      <c r="E42" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="5:5" ht="14.7">
-      <c r="E43" s="12"/>
-    </row>
-    <row r="44" spans="5:5">
-      <c r="E44" s="6" t="s">
+    <row r="51" spans="5:5" ht="17.100000000000001">
+      <c r="E51" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5">
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" spans="5:5">
+      <c r="E53" s="11"/>
+    </row>
+    <row r="54" spans="5:5">
+      <c r="E54" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5">
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="5:5">
+      <c r="E56" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="5:5">
+      <c r="E57" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5">
+      <c r="E58" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="5:5">
+      <c r="E59" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="5:5">
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="5:5">
+      <c r="E61" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="5:5">
+      <c r="E62" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="5:5" ht="17.100000000000001">
-      <c r="E45" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="5:5">
-      <c r="E46" s="13"/>
-    </row>
-    <row r="47" spans="5:5">
-      <c r="E47" s="13"/>
-    </row>
-    <row r="48" spans="5:5">
-      <c r="E48" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="5:5">
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="5:5">
-      <c r="E50" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="5:5">
-      <c r="E51" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="5:5">
-      <c r="E52" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="5:5">
-      <c r="E53" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="5:5">
-      <c r="E54" s="6"/>
-    </row>
-    <row r="55" spans="5:5">
-      <c r="E55" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="5:5">
-      <c r="E56" s="6" t="s">
+    <row r="63" spans="5:5">
+      <c r="E63" s="5" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="5:5">
-      <c r="E57" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>